<commit_message>
Updated plots after last run, so we have all results updated
</commit_message>
<xml_diff>
--- a/collapsed_grouped_words_table_colored.xlsx
+++ b/collapsed_grouped_words_table_colored.xlsx
@@ -511,36 +511,36 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Legal Entity</t>
+          <t>Geographic Distance</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>&lt;span style="color:#e78ac3"&gt;Dashti&lt;/span&gt;, &lt;span style="color:#fc8d62"&gt;Britto_2016&lt;/span&gt;</t>
+          <t>&lt;span style="color:#fc8d62"&gt;Britto_2016&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Geographic Distance</t>
+          <t>Temporal Distance</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>&lt;span style="color:#fc8d62"&gt;Britto_2016&lt;/span&gt;</t>
+          <t>&lt;span style="color:#fc8d62"&gt;Britto_2016&lt;/span&gt;, &lt;span style="color:#66c2a5"&gt;Bajta&lt;/span&gt;</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Temporal Distance</t>
+          <t>Legal Entity</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>&lt;span style="color:#fc8d62"&gt;Britto_2016&lt;/span&gt;, &lt;span style="color:#66c2a5"&gt;Bajta&lt;/span&gt;</t>
+          <t>&lt;span style="color:#fc8d62"&gt;Britto_2016&lt;/span&gt;, &lt;span style="color:#e78ac3"&gt;Dashti&lt;/span&gt;</t>
         </is>
       </c>
     </row>

</xml_diff>